<commit_message>
general director add columns
</commit_message>
<xml_diff>
--- a/companies_data.xlsx
+++ b/companies_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>ИНН</t>
   </si>
@@ -22,6 +22,12 @@
     <t>Дата регистрации</t>
   </si>
   <si>
+    <t>Ген. директор</t>
+  </si>
+  <si>
+    <t>Учредитель</t>
+  </si>
+  <si>
     <t>Телефон</t>
   </si>
   <si>
@@ -34,127 +40,85 @@
     <t>Дата добавления</t>
   </si>
   <si>
-    <t>9403033090</t>
-  </si>
-  <si>
-    <t>9405004384</t>
-  </si>
-  <si>
-    <t>9403033083</t>
-  </si>
-  <si>
-    <t>9200028105</t>
-  </si>
-  <si>
-    <t>9200028095</t>
-  </si>
-  <si>
-    <t>9200028070</t>
-  </si>
-  <si>
-    <t>9109033498</t>
-  </si>
-  <si>
-    <t>9109033480</t>
-  </si>
-  <si>
-    <t>9110035820</t>
-  </si>
-  <si>
-    <t>9103106816</t>
-  </si>
-  <si>
-    <t>28 мая 2025 года</t>
-  </si>
-  <si>
-    <t>dobryiput2025@mail.ru</t>
-  </si>
-  <si>
-    <t>horizon_severodonetsk@mail.ru</t>
-  </si>
-  <si>
-    <t>centrlisenartlnr@mail.ru</t>
-  </si>
-  <si>
-    <t>irbnsev@mail.ru</t>
-  </si>
-  <si>
-    <t>dinastiya.sev@mail.ru</t>
-  </si>
-  <si>
-    <t>triumfgym@mail.ru</t>
-  </si>
-  <si>
-    <t>vozrojdenie2026@bk.ru</t>
-  </si>
-  <si>
-    <t>alimovmamut@mail.ru</t>
-  </si>
-  <si>
-    <t>ismet-87@mail.ru</t>
-  </si>
-  <si>
-    <t>oookupazhooo@gmail.com</t>
-  </si>
-  <si>
-    <t>https://checko.ru/company/dobry-put-1259400002630</t>
-  </si>
-  <si>
-    <t>https://checko.ru/company/gorizont-1259400002620</t>
-  </si>
-  <si>
-    <t>https://checko.ru/company/aclavl-1259400002608</t>
-  </si>
-  <si>
-    <t>https://checko.ru/company/irbn-1259200002467</t>
-  </si>
-  <si>
-    <t>https://checko.ru/company/dinastiya-1259200002456</t>
-  </si>
-  <si>
-    <t>https://checko.ru/company/rofso-fssgs-1259200002434</t>
-  </si>
-  <si>
-    <t>https://checko.ru/company/vozrozhdenie-1259100007770</t>
-  </si>
-  <si>
-    <t>https://checko.ru/company/limamarket-1259100007760</t>
-  </si>
-  <si>
-    <t>https://checko.ru/company/kfh-dort-1259100007748</t>
-  </si>
-  <si>
-    <t>https://checko.ru/company/kupazh-1259100007737</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:29:00</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:29:04</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:29:09</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:29:13</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:29:19</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:29:24</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:29:29</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:29:34</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:29:40</t>
-  </si>
-  <si>
-    <t>2025-05-29 17:29:45</t>
+    <t>EmailSent</t>
+  </si>
+  <si>
+    <t>7804715509</t>
+  </si>
+  <si>
+    <t>7807399192</t>
+  </si>
+  <si>
+    <t>9717179911</t>
+  </si>
+  <si>
+    <t>9703212936</t>
+  </si>
+  <si>
+    <t>9707047183</t>
+  </si>
+  <si>
+    <t>29 мая 2025 года</t>
+  </si>
+  <si>
+    <t>Меланин Евгений Валерьевич</t>
+  </si>
+  <si>
+    <t>Блинов Николай Ильич</t>
+  </si>
+  <si>
+    <t>Силантьев Павел Витальевич</t>
+  </si>
+  <si>
+    <t>Ерохин Александр Сергеевич</t>
+  </si>
+  <si>
+    <t>Филиппова Ольга Александровна</t>
+  </si>
+  <si>
+    <t>metrologia2050@yandex.ru</t>
+  </si>
+  <si>
+    <t>oooruspitavto@mail.ru</t>
+  </si>
+  <si>
+    <t>nblinov.1997@bk.ru</t>
+  </si>
+  <si>
+    <t>silatech@bk.ru</t>
+  </si>
+  <si>
+    <t>russian-steel@mail.ru</t>
+  </si>
+  <si>
+    <t>https://checko.ru/company/metrologiya-2050-1257800048978</t>
+  </si>
+  <si>
+    <t>https://checko.ru/company/ruspitavto-1257800048912</t>
+  </si>
+  <si>
+    <t>https://checko.ru/company/rsk-1257700242964</t>
+  </si>
+  <si>
+    <t>https://checko.ru/company/realtrans-1257700243239</t>
+  </si>
+  <si>
+    <t>https://checko.ru/company/russkaya-stal-1257700243338</t>
+  </si>
+  <si>
+    <t>2025-05-30 11:31:54</t>
+  </si>
+  <si>
+    <t>2025-05-30 11:31:57</t>
+  </si>
+  <si>
+    <t>2025-05-30 11:32:01</t>
+  </si>
+  <si>
+    <t>2025-05-30 11:32:06</t>
+  </si>
+  <si>
+    <t>2025-05-30 11:32:11</t>
   </si>
 </sst>
 </file>
@@ -525,20 +489,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="3" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
+    <col min="8" max="9" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,189 +522,150 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>37</v>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="H6" t="s">
         <v>34</v>
       </c>
-      <c r="F9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" t="s">
-        <v>46</v>
+      <c r="I6" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>